<commit_message>
update content and fix page width at small screen sizes
</commit_message>
<xml_diff>
--- a/src/_data/june-2023-translated-final.xlsx
+++ b/src/_data/june-2023-translated-final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\nina\new\mybus-v3\src\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147EBBB5-138D-45E1-B5B7-9C844F33B751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4B9AE4-A934-428E-91EA-D18D026157C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20430" yWindow="-8820" windowWidth="19950" windowHeight="19740" activeTab="1" xr2:uid="{74382335-5AEE-466B-91D9-2624957AED8F}"/>
+    <workbookView xWindow="435" yWindow="570" windowWidth="19950" windowHeight="19740" xr2:uid="{74382335-5AEE-466B-91D9-2624957AED8F}"/>
   </bookViews>
   <sheets>
     <sheet name="updates" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2168" uniqueCount="791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2237" uniqueCount="797">
   <si>
     <t>Line 78 adjusted to operate every 20 minutes on weekends</t>
   </si>
@@ -2411,6 +2411,24 @@
   </si>
   <si>
     <t>Harbor Gateway Transit Center to El Monte Station</t>
+  </si>
+  <si>
+    <t>languages</t>
+  </si>
+  <si>
+    <t>Back to top</t>
+  </si>
+  <si>
+    <t>backToTop</t>
+  </si>
+  <si>
+    <t>Languages</t>
+  </si>
+  <si>
+    <t>downloadSummary</t>
+  </si>
+  <si>
+    <t>Download Summary</t>
   </si>
 </sst>
 </file>
@@ -3453,8 +3471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F1E7A70-D752-42E3-8C5C-5A7AA7A09360}">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4323,13 +4341,27 @@
       <c r="M15" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="N15" s="12"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="12"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="12"/>
+      <c r="N15" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="O15" t="s">
+        <v>563</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>565</v>
+      </c>
+      <c r="R15" t="s">
+        <v>566</v>
+      </c>
+      <c r="S15" t="s">
+        <v>567</v>
+      </c>
+      <c r="T15" s="6" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
@@ -4472,13 +4504,27 @@
       <c r="M18" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="N18" s="12"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="12"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="12"/>
+      <c r="N18" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="O18" t="s">
+        <v>563</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>565</v>
+      </c>
+      <c r="R18" t="s">
+        <v>566</v>
+      </c>
+      <c r="S18" t="s">
+        <v>567</v>
+      </c>
+      <c r="T18" s="6" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
@@ -7701,13 +7747,27 @@
       <c r="M73" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="N73" s="12"/>
-      <c r="O73" s="9"/>
-      <c r="P73" s="12"/>
-      <c r="Q73" s="9"/>
-      <c r="R73" s="12"/>
-      <c r="S73" s="9"/>
-      <c r="T73" s="12"/>
+      <c r="N73" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="O73" t="s">
+        <v>563</v>
+      </c>
+      <c r="P73" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>565</v>
+      </c>
+      <c r="R73" t="s">
+        <v>566</v>
+      </c>
+      <c r="S73" t="s">
+        <v>567</v>
+      </c>
+      <c r="T73" s="6" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="13">
@@ -8027,13 +8087,27 @@
       <c r="M79" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="N79" s="12"/>
-      <c r="O79" s="9"/>
-      <c r="P79" s="12"/>
-      <c r="Q79" s="9"/>
-      <c r="R79" s="12"/>
-      <c r="S79" s="9"/>
-      <c r="T79" s="12"/>
+      <c r="N79" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="O79" t="s">
+        <v>563</v>
+      </c>
+      <c r="P79" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>565</v>
+      </c>
+      <c r="R79" t="s">
+        <v>566</v>
+      </c>
+      <c r="S79" t="s">
+        <v>567</v>
+      </c>
+      <c r="T79" s="6" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="13">
@@ -9068,13 +9142,27 @@
       <c r="M97" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="N97" s="12"/>
-      <c r="O97" s="9"/>
-      <c r="P97" s="12"/>
-      <c r="Q97" s="9"/>
-      <c r="R97" s="12"/>
-      <c r="S97" s="9"/>
-      <c r="T97" s="12"/>
+      <c r="N97" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="O97" t="s">
+        <v>563</v>
+      </c>
+      <c r="P97" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>565</v>
+      </c>
+      <c r="R97" t="s">
+        <v>566</v>
+      </c>
+      <c r="S97" t="s">
+        <v>567</v>
+      </c>
+      <c r="T97" s="6" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" s="13">
@@ -9279,13 +9367,27 @@
       <c r="M101" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="N101" s="12"/>
-      <c r="O101" s="9"/>
-      <c r="P101" s="12"/>
-      <c r="Q101" s="9"/>
-      <c r="R101" s="12"/>
-      <c r="S101" s="9"/>
-      <c r="T101" s="12"/>
+      <c r="N101" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="O101" t="s">
+        <v>563</v>
+      </c>
+      <c r="P101" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>565</v>
+      </c>
+      <c r="R101" t="s">
+        <v>566</v>
+      </c>
+      <c r="S101" t="s">
+        <v>567</v>
+      </c>
+      <c r="T101" s="6" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" s="13">
@@ -9369,13 +9471,27 @@
       <c r="M103" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="N103" s="12"/>
-      <c r="O103" s="9"/>
-      <c r="P103" s="12"/>
-      <c r="Q103" s="9"/>
-      <c r="R103" s="12"/>
-      <c r="S103" s="9"/>
-      <c r="T103" s="12"/>
+      <c r="N103" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="O103" t="s">
+        <v>563</v>
+      </c>
+      <c r="P103" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>565</v>
+      </c>
+      <c r="R103" t="s">
+        <v>566</v>
+      </c>
+      <c r="S103" t="s">
+        <v>567</v>
+      </c>
+      <c r="T103" s="6" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" s="17">
@@ -9400,13 +9516,27 @@
       <c r="M104" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="N104" s="12"/>
-      <c r="O104" s="9"/>
-      <c r="P104" s="12"/>
-      <c r="Q104" s="9"/>
-      <c r="R104" s="12"/>
-      <c r="S104" s="9"/>
-      <c r="T104" s="12"/>
+      <c r="N104" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="O104" t="s">
+        <v>563</v>
+      </c>
+      <c r="P104" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>565</v>
+      </c>
+      <c r="R104" t="s">
+        <v>566</v>
+      </c>
+      <c r="S104" t="s">
+        <v>567</v>
+      </c>
+      <c r="T104" s="6" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" s="13">
@@ -9490,13 +9620,27 @@
       <c r="M106" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="N106" s="12"/>
-      <c r="O106" s="9"/>
-      <c r="P106" s="12"/>
-      <c r="Q106" s="9"/>
-      <c r="R106" s="12"/>
-      <c r="S106" s="9"/>
-      <c r="T106" s="12"/>
+      <c r="N106" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="O106" t="s">
+        <v>563</v>
+      </c>
+      <c r="P106" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>565</v>
+      </c>
+      <c r="R106" t="s">
+        <v>566</v>
+      </c>
+      <c r="S106" t="s">
+        <v>567</v>
+      </c>
+      <c r="T106" s="6" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" s="13">
@@ -9689,7 +9833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F8B66C-CC82-4391-A0D4-0A06AC267444}">
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
@@ -10966,15 +11110,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E787A09F-AFB1-4A95-B59A-5923C3270ABC}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" customWidth="1"/>
   </cols>
@@ -11419,6 +11563,30 @@
         <v>757</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>791</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>795</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>793</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>792</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add urls to rail line icons to data
</commit_message>
<xml_diff>
--- a/src/_data/june-2023-translated-final.xlsx
+++ b/src/_data/june-2023-translated-final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\nina\new\mybus-v3\src\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F511FCF-4D33-4A5C-8F7D-F26A8FA8ED81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0532FB1C-A7E9-48D1-A07A-85420F997D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{74382335-5AEE-466B-91D9-2624957AED8F}"/>
+    <workbookView xWindow="330" yWindow="750" windowWidth="17178" windowHeight="11022" activeTab="1" xr2:uid="{74382335-5AEE-466B-91D9-2624957AED8F}"/>
   </bookViews>
   <sheets>
     <sheet name="updates" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2303" uniqueCount="800">
   <si>
     <t>Line 78 adjusted to operate every 20 minutes on weekends</t>
   </si>
@@ -2429,13 +2429,22 @@
   </si>
   <si>
     <t>Select Language</t>
+  </si>
+  <si>
+    <t>icon_url</t>
+  </si>
+  <si>
+    <t>https://lacmta.github.io/metro-iconography/Service_ALine.svg</t>
+  </si>
+  <si>
+    <t>https://lacmta.github.io/metro-iconography/Service_KLine.svg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2485,6 +2494,14 @@
       <color rgb="FF374151"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2532,10 +2549,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2598,8 +2616,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="25">
@@ -3169,13 +3189,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6B6FBED3-A523-4AA3-B67B-B7AC18364AAF}" name="Table3" displayName="Table3" ref="A1:D99" totalsRowShown="0">
-  <autoFilter ref="A1:D99" xr:uid="{6B6FBED3-A523-4AA3-B67B-B7AC18364AAF}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6B6FBED3-A523-4AA3-B67B-B7AC18364AAF}" name="Table3" displayName="Table3" ref="A1:E99" totalsRowShown="0">
+  <autoFilter ref="A1:E99" xr:uid="{6B6FBED3-A523-4AA3-B67B-B7AC18364AAF}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B598E7EA-51CE-4662-8C3C-CF6FC7A355C3}" name="line"/>
     <tableColumn id="2" xr3:uid="{1B7E6D09-ECC4-47A0-BC0F-BAC452B20F27}" name="schedule"/>
     <tableColumn id="3" xr3:uid="{27AEDE00-3BA8-457B-A7DF-902155D65A4F}" name="line_label" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{2DCFB644-D2A4-43D0-B00E-E9A232611936}" name="description"/>
+    <tableColumn id="5" xr3:uid="{864EF5D8-629B-47F5-8520-0E52B0D5CC37}" name="icon_url"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3480,7 +3501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F1E7A70-D752-42E3-8C5C-5A7AA7A09360}">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+    <sheetView topLeftCell="B31" workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -9966,10 +9987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F8B66C-CC82-4391-A0D4-0A06AC267444}">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -9980,7 +10001,7 @@
     <col min="4" max="4" width="63" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>107</v>
       </c>
@@ -9993,8 +10014,11 @@
       <c r="D1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E1" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>2</v>
       </c>
@@ -10008,7 +10032,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>4</v>
       </c>
@@ -10022,7 +10046,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>10</v>
       </c>
@@ -10036,7 +10060,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>14</v>
       </c>
@@ -10050,7 +10074,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>16</v>
       </c>
@@ -10064,7 +10088,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>18</v>
       </c>
@@ -10078,7 +10102,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>20</v>
       </c>
@@ -10092,7 +10116,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>28</v>
       </c>
@@ -10106,7 +10130,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>30</v>
       </c>
@@ -10120,7 +10144,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>33</v>
       </c>
@@ -10134,7 +10158,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>37</v>
       </c>
@@ -10148,7 +10172,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>40</v>
       </c>
@@ -10162,7 +10186,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>45</v>
       </c>
@@ -10176,7 +10200,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>48</v>
       </c>
@@ -10190,7 +10214,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>51</v>
       </c>
@@ -11097,7 +11121,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A81">
         <v>665</v>
       </c>
@@ -11111,7 +11135,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A82">
         <v>720</v>
       </c>
@@ -11125,7 +11149,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A83">
         <v>754</v>
       </c>
@@ -11139,7 +11163,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A84">
         <v>761</v>
       </c>
@@ -11153,7 +11177,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A85">
         <v>802</v>
       </c>
@@ -11166,8 +11190,11 @@
       <c r="D85" t="s">
         <v>781</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E85" s="22" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A86">
         <v>807</v>
       </c>
@@ -11180,8 +11207,11 @@
       <c r="D86" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E86" s="22" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A87">
         <v>854</v>
       </c>
@@ -11192,7 +11222,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A88">
         <v>857</v>
       </c>
@@ -11206,7 +11236,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A89">
         <v>901</v>
       </c>
@@ -11219,8 +11249,9 @@
       <c r="D89" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E89" s="22"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A90">
         <v>910</v>
       </c>
@@ -11236,9 +11267,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E85" r:id="rId1" xr:uid="{158A7C20-61C5-46AF-8A6A-B2DD39672ABD}"/>
+    <hyperlink ref="E86" r:id="rId2" xr:uid="{AC905C0C-C82D-4FC2-98BB-74D5DA172210}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fix: wrong date on `L line`
</commit_message>
<xml_diff>
--- a/src/_data/june-2023-translated-final.xlsx
+++ b/src/_data/june-2023-translated-final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kochaphuma\repos\metro\mybus-v3\src\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE62F39-13AC-47C1-97C0-8C154BE0DB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6688D9-81CC-456E-84EB-8F2BEF02406C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="18915" windowHeight="12075" xr2:uid="{74382335-5AEE-466B-91D9-2624957AED8F}"/>
   </bookViews>
@@ -2438,7 +2438,7 @@
     <t>https://lacmta.github.io/metro-iconography/Service_BLine.svg</t>
   </si>
   <si>
-    <t>The L Line Shuttle between LA Union Station and Pico Aliso Station will cease operation on Saturday, June 18.</t>
+    <t>The L Line Shuttle between LA Union Station and Pico Aliso Station will cease operation on Saturday, June 17.</t>
   </si>
 </sst>
 </file>
@@ -3503,7 +3503,7 @@
   <dimension ref="A1:T109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+      <selection activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>